<commit_message>
Updates and switched back to damn Excel heatmap
</commit_message>
<xml_diff>
--- a/draft/supplemental_fig/heatmap.xlsx
+++ b/draft/supplemental_fig/heatmap.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="0" windowWidth="35560" windowHeight="21080" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="219">
   <si>
     <t>sample</t>
   </si>
@@ -689,7 +689,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode=";;;"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -714,43 +714,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Source Code Pro"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="28"/>
-      <name val="Source Code Pro"/>
-    </font>
-    <font>
-      <sz val="28"/>
-      <color theme="1"/>
-      <name val="Source Code Pro"/>
-    </font>
-    <font>
-      <sz val="28"/>
-      <name val="Source Code Pro"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <color theme="1"/>
-      <name val="Source Code Pro"/>
     </font>
     <font>
       <b/>
@@ -761,9 +728,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="128"/>
+      <sz val="28"/>
       <color theme="1"/>
-      <name val="Source Code Pro"/>
+      <name val="Myriad Pro"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <name val="Myriad Pro"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <name val="Myriad Pro"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Myriad Pro"/>
     </font>
   </fonts>
   <fills count="2">
@@ -831,30 +813,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="180"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1230,1449 +1206,1401 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N110"/>
+  <dimension ref="B1:M103"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="37" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="35" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="1" customWidth="1"/>
-    <col min="2" max="4" width="28.83203125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="1.33203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="38.83203125" style="5" customWidth="1"/>
+    <col min="2" max="4" width="5.5" style="6" customWidth="1"/>
+    <col min="5" max="5" width="1.33203125" style="6" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="4"/>
-    <col min="7" max="7" width="69.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="69.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="129.75" customHeight="1">
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+    <row r="1" spans="2:13" ht="129.75" customHeight="1">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="2:14" ht="162">
-      <c r="B2" s="5">
+    <row r="2" spans="2:13">
+      <c r="B2" s="6">
         <v>-0.44130228669316729</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="6">
         <v>-0.20464671950873381</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <v>-0.64594642082365272</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="H2" s="5">
-        <v>1</v>
-      </c>
-      <c r="I2" s="9">
-        <v>1</v>
-      </c>
-      <c r="J2"/>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7">
+        <v>1</v>
+      </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
-      <c r="N2"/>
-    </row>
-    <row r="3" spans="2:14" ht="162">
-      <c r="B3" s="5">
+    </row>
+    <row r="3" spans="2:13">
+      <c r="B3" s="6">
         <v>-0.75893154417661002</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="6">
         <v>-0.43432080663704675</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="6">
         <v>-1.1932511226035434</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="6">
         <v>0.5</v>
       </c>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="2:14" ht="162">
-      <c r="B4" s="5">
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="B4" s="6">
         <v>-0.13959423549425587</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="6">
         <v>-0.1527038520172006</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <v>-0.29229837696333849</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="6">
         <v>0.25</v>
       </c>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="2:14" ht="162">
-      <c r="B5" s="5">
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="2:13">
+      <c r="B5" s="6">
         <v>-1.8056412756359386E-2</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="6">
         <v>-0.55536449936182253</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <v>-0.57341814749162889</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="6">
         <v>0</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="162">
-      <c r="B6" s="5">
+    <row r="6" spans="2:13">
+      <c r="B6" s="6">
         <v>-0.65198603885148021</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="6">
         <v>-0.78650332474840923</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <v>-1.4384859308548541</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="6">
         <v>-1.25</v>
       </c>
-      <c r="I6" s="10"/>
-    </row>
-    <row r="7" spans="2:14" ht="162">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5">
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="6">
         <v>-4.7575225530421061</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="6">
         <v>-2.5</v>
       </c>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" spans="2:14" ht="162">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5">
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="2:13" ht="36">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="6">
         <v>-4.331553820769825</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="6">
         <v>-5</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="7">
         <v>-5</v>
       </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="2:14" ht="162">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5">
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="6">
         <v>-4.53567380342575</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="2:14" ht="162">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="F10" s="12" t="s">
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="2:13">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="F10" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="2:14" ht="162">
-      <c r="B11" s="5">
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="2:13">
+      <c r="B11" s="6">
         <v>-0.10949552795352258</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="6">
         <v>-0.20464671950873381</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="6">
         <v>-0.31413959689263216</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="2:14" ht="162">
-      <c r="B12" s="5">
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="B12" s="6">
         <v>-0.15899179049465806</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="6">
         <v>-2.618009729223969E-2</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="6">
         <v>-0.18516993693403894</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="162">
-      <c r="B13" s="5">
+    <row r="13" spans="2:13">
+      <c r="B13" s="6">
         <v>-2.5314789170422554</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="6">
         <v>-0.41852653945381491</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="6">
         <v>-2.9490864987539949</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="2:14" ht="162">
-      <c r="B14" s="5">
+    <row r="14" spans="2:13">
+      <c r="B14" s="6">
         <v>-1.9081901974049575E-2</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="6">
         <v>-0.11491529112780086</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="6">
         <v>-0.13399760761628876</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="2:14" ht="162">
-      <c r="B15" s="5">
+    <row r="15" spans="2:13">
+      <c r="B15" s="6">
         <v>7.8853600251697298E-2</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="6">
         <v>-0.31349863622357899</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="6">
         <v>-0.23464380776176874</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="162">
-      <c r="B16" s="5">
+    <row r="16" spans="2:13">
+      <c r="B16" s="6">
         <v>-2.6676986640602443</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="6">
         <v>-0.65368075584970842</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="6">
         <v>-3.320829955378052</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="162">
-      <c r="B17" s="5">
+    <row r="17" spans="2:6">
+      <c r="B17" s="6">
         <v>-0.79111622754801125</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="6">
         <v>-0.46716971825197828</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="6">
         <v>-1.2582938287584953</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="162">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="5">
+    <row r="18" spans="2:6">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="6">
         <v>-4.7575225530421061</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="162">
-      <c r="B19" s="5">
+    <row r="19" spans="2:6">
+      <c r="B19" s="6">
         <v>-1.021656269215161</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="6">
         <v>-1.238557625334932</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="6">
         <v>-2.2601321150244402</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="162">
-      <c r="B20" s="5">
+    <row r="20" spans="2:6">
+      <c r="B20" s="6">
         <v>-0.27251026637898512</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="6">
         <v>-0.49501864699065856</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="6">
         <v>-0.76752428074579182</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="162">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="12" t="s">
+    <row r="21" spans="2:6">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="162">
-      <c r="B22" s="5">
+    <row r="22" spans="2:6">
+      <c r="B22" s="6">
         <v>-2.2836944333314992</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="6">
         <v>-9.7752485594076788E-2</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="6">
         <v>-2.381554277909903</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="162">
-      <c r="B23" s="5">
+    <row r="23" spans="2:6">
+      <c r="B23" s="6">
         <v>-2.957749106970553E-3</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="6">
         <v>0.17273113024841447</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="6">
         <v>0.16977422353168681</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="162">
-      <c r="B24" s="5">
+    <row r="24" spans="2:6">
+      <c r="B24" s="6">
         <v>-2.1203774623122467</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="6">
         <v>-0.36373973235133961</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="6">
         <v>-2.4841354129104225</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="162">
-      <c r="B25" s="5">
+    <row r="25" spans="2:6">
+      <c r="B25" s="6">
         <v>-1.8672710189654482</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="6">
         <v>-0.47003635890358142</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="6">
         <v>-2.3375668045523486</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="162">
-      <c r="B26" s="5">
+    <row r="26" spans="2:6">
+      <c r="B26" s="6">
         <v>-1.5348325590498428</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="6">
         <v>-2.2192057497195883E-2</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="6">
         <v>-1.5570368550412756</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="162">
-      <c r="B27" s="5">
+    <row r="27" spans="2:6">
+      <c r="B27" s="6">
         <v>-3.6454222693490919</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="6">
         <v>0.70748585525854857</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="6">
         <v>-2.9379786175002378</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="162">
-      <c r="B28" s="5">
+    <row r="28" spans="2:6">
+      <c r="B28" s="6">
         <v>-1.5232063910762652</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="6">
         <v>0.31386722036915371</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="6">
         <v>-1.2093379424969983</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="162">
-      <c r="B29" s="5">
+    <row r="29" spans="2:6">
+      <c r="B29" s="6">
         <v>-0.26611675159850989</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="6">
         <v>-0.45254562674324594</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="6">
         <v>-0.71866405148234058</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="162">
-      <c r="B30" s="5">
+    <row r="30" spans="2:6">
+      <c r="B30" s="6">
         <v>-0.24402172856754767</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="6">
         <v>1.9842126273831084E-2</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="6">
         <v>-0.22417847748706432</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="162">
-      <c r="B31" s="5">
+    <row r="31" spans="2:6">
+      <c r="B31" s="6">
         <v>-0.34114721887196353</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="6">
         <v>0.18546795165134711</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="6">
         <v>-0.15567976326000821</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="162">
-      <c r="B32" s="5">
+    <row r="32" spans="2:6">
+      <c r="B32" s="6">
         <v>-3.9578730291002895E-2</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="6">
         <v>-0.33351574974546616</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="6">
         <v>-0.37309147590459624</v>
       </c>
-      <c r="F32" s="12" t="s">
+      <c r="F32" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="162">
-      <c r="B33" s="5">
+    <row r="33" spans="2:6">
+      <c r="B33" s="6">
         <v>-4.2819748928835555E-2</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="6">
         <v>0.15671278046287229</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="6">
         <v>0.11389469349622505</v>
       </c>
-      <c r="F33" s="12" t="s">
+      <c r="F33" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="162">
-      <c r="B34" s="5">
+    <row r="34" spans="2:6">
+      <c r="B34" s="6">
         <v>-0.20215928189039678</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="6">
         <v>-7.9883419978926895E-2</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="6">
         <v>-0.2820402294659905</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="162">
-      <c r="B35" s="5">
+    <row r="35" spans="2:6">
+      <c r="B35" s="6">
         <v>-0.12037746231224666</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="6">
         <v>-0.16209436882327033</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="6">
         <v>-0.28247153633544286</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F35" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="2:6" ht="162">
-      <c r="B36" s="5">
+    <row r="36" spans="2:6">
+      <c r="B36" s="6">
         <v>4.7424649928137885E-2</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="6">
         <v>-6.4893954947219612E-2</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="6">
         <v>-1.7467927052276622E-2</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F36" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="2:6" ht="162">
-      <c r="B37" s="5">
+    <row r="37" spans="2:6">
+      <c r="B37" s="6">
         <v>-0.89337382152965361</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="6">
         <v>-0.17298813490778997</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="6">
         <v>-1.0663526189105026</v>
       </c>
-      <c r="F37" s="12" t="s">
+      <c r="F37" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="2:6" ht="162">
-      <c r="B38" s="5">
+    <row r="38" spans="2:6">
+      <c r="B38" s="6">
         <v>2.9438871388719701E-2</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="6">
         <v>5.0894467044324543E-3</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D38" s="6">
         <v>3.4530441518240806E-2</v>
       </c>
-      <c r="F38" s="12" t="s">
+      <c r="F38" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="2:6" ht="162">
-      <c r="B39" s="5">
+    <row r="39" spans="2:6">
+      <c r="B39" s="6">
         <v>-0.27993428445819246</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="6">
         <v>-0.10177375952700096</v>
       </c>
-      <c r="D39" s="5">
+      <c r="D39" s="6">
         <v>-0.38170658178027139</v>
       </c>
-      <c r="F39" s="12" t="s">
+      <c r="F39" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="2:6" ht="162">
-      <c r="B40" s="5">
+    <row r="40" spans="2:6">
+      <c r="B40" s="6">
         <v>-0.64759918860336629</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="6">
         <v>-0.18416750331787357</v>
       </c>
-      <c r="D40" s="5">
+      <c r="D40" s="6">
         <v>-0.8317636741596619</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F40" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="2:6" ht="162">
-      <c r="B41" s="5">
+    <row r="41" spans="2:6">
+      <c r="B41" s="6">
         <v>-0.85654715357367506</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="6">
         <v>8.4411004591533612E-4</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D41" s="6">
         <v>-0.85570110914833108</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F41" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="162">
-      <c r="B42" s="5">
+    <row r="42" spans="2:6">
+      <c r="B42" s="6">
         <v>-0.3389972417984044</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="6">
         <v>-0.30102999566398103</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42" s="6">
         <v>-0.64003029860167082</v>
       </c>
-      <c r="F42" s="12" t="s">
+      <c r="F42" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="43" spans="2:6" ht="162">
-      <c r="B43" s="5">
+    <row r="43" spans="2:6">
+      <c r="B43" s="6">
         <v>-0.20846493867964222</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="6">
         <v>-8.4072788302884227E-2</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D43" s="6">
         <v>-0.29253649877241283</v>
       </c>
-      <c r="F43" s="12" t="s">
+      <c r="F43" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="162">
-      <c r="B44" s="5">
+    <row r="44" spans="2:6">
+      <c r="B44" s="6">
         <v>-1.8782664032669114</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="6">
         <v>-0.55301059396834518</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D44" s="6">
         <v>-2.4311866921133549</v>
       </c>
-      <c r="F44" s="12" t="s">
+      <c r="F44" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="162">
-      <c r="B45" s="5">
+    <row r="45" spans="2:6">
+      <c r="B45" s="6">
         <v>-1.3201118976380308</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C45" s="6">
         <v>0.3173555482149748</v>
       </c>
-      <c r="D45" s="5">
+      <c r="D45" s="6">
         <v>-1.0027666204152901</v>
       </c>
-      <c r="F45" s="12" t="s">
+      <c r="F45" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="2:6" ht="162">
-      <c r="B46" s="5">
+    <row r="46" spans="2:6">
+      <c r="B46" s="6">
         <v>-0.99269257327984439</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="6">
         <v>0.91246667958760952</v>
       </c>
-      <c r="D46" s="5">
+      <c r="D46" s="6">
         <v>-7.7459125560157993E-2</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="F46" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="162">
-      <c r="B47" s="5">
+    <row r="47" spans="2:6">
+      <c r="B47" s="6">
         <v>-0.91302850952612324</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="6">
         <v>-0.14672996852844777</v>
       </c>
-      <c r="D47" s="5">
+      <c r="D47" s="6">
         <v>-1.0597702788743515</v>
       </c>
-      <c r="F47" s="12" t="s">
+      <c r="F47" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="48" spans="2:6" ht="162">
-      <c r="B48" s="5">
+    <row r="48" spans="2:6">
+      <c r="B48" s="6">
         <v>-0.74233228235714854</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="6">
         <v>-0.21965064164781367</v>
       </c>
-      <c r="D48" s="5">
+      <c r="D48" s="6">
         <v>-0.9619901103319517</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="F48" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="162">
-      <c r="B49" s="5">
+    <row r="49" spans="2:6">
+      <c r="B49" s="6">
         <v>-0.1216758025375273</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C49" s="6">
         <v>-0.37455260163355697</v>
       </c>
-      <c r="D49" s="5">
+      <c r="D49" s="6">
         <v>-0.49622795613140003</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="F49" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="162">
-      <c r="B50" s="5">
+    <row r="50" spans="2:6">
+      <c r="B50" s="6">
         <v>-0.75893154417661002</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C50" s="6">
         <v>-0.57149399966235848</v>
       </c>
-      <c r="D50" s="5">
+      <c r="D50" s="6">
         <v>-1.3304152914216902</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F50" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="162">
-      <c r="B51" s="5">
+    <row r="51" spans="2:6">
+      <c r="B51" s="6">
         <v>-0.49620315669371218</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C51" s="6">
         <v>-0.32161652644575844</v>
       </c>
-      <c r="D51" s="5">
+      <c r="D51" s="6">
         <v>-0.81782030299491471</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="F51" s="4" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="162">
-      <c r="B52" s="5">
+    <row r="52" spans="2:6">
+      <c r="B52" s="6">
         <v>6.8240716542313784E-3</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C52" s="6">
         <v>-0.53616603732061541</v>
       </c>
-      <c r="D52" s="5">
+      <c r="D52" s="6">
         <v>-0.52934470319236393</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F52" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="53" spans="2:6" ht="162">
-      <c r="B53" s="5">
+    <row r="53" spans="2:6">
+      <c r="B53" s="6">
         <v>1.0949404201451522</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C53" s="6">
         <v>-0.57822738232132687</v>
       </c>
-      <c r="D53" s="5">
+      <c r="D53" s="6">
         <v>0.51671460162499905</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F53" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="2:6" ht="162">
-      <c r="B54" s="5">
+    <row r="54" spans="2:6">
+      <c r="B54" s="6">
         <v>-0.51348297413866728</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C54" s="6">
         <v>0.37936876912558581</v>
       </c>
-      <c r="D54" s="5">
+      <c r="D54" s="6">
         <v>-0.13411129411543143</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F54" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="2:6" ht="162">
-      <c r="B55" s="5">
+    <row r="55" spans="2:6">
+      <c r="B55" s="6">
         <v>-0.25009587627974117</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C55" s="6">
         <v>-6.4167102088177774E-2</v>
       </c>
-      <c r="D55" s="5">
+      <c r="D55" s="6">
         <v>-0.31425956558341106</v>
       </c>
-      <c r="F55" s="12" t="s">
+      <c r="F55" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="56" spans="2:6" ht="162">
-      <c r="B56" s="5">
+    <row r="56" spans="2:6">
+      <c r="B56" s="6">
         <v>-1.1568715528486477</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C56" s="6">
         <v>-0.29251414474145143</v>
       </c>
-      <c r="D56" s="5">
+      <c r="D56" s="6">
         <v>-1.4493851744040676</v>
       </c>
-      <c r="F56" s="12" t="s">
+      <c r="F56" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="57" spans="2:6" ht="162">
-      <c r="B57" s="5">
+    <row r="57" spans="2:6">
+      <c r="B57" s="6">
         <v>-0.37825054094607813</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C57" s="6">
         <v>-0.27406812826720239</v>
       </c>
-      <c r="D57" s="5">
+      <c r="D57" s="6">
         <v>-0.65231903733176466</v>
       </c>
-      <c r="F57" s="12" t="s">
+      <c r="F57" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="2:6" ht="162">
-      <c r="B58" s="5">
+    <row r="58" spans="2:6">
+      <c r="B58" s="6">
         <v>-1.8426485440571163</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C58" s="6">
         <v>-0.27361924504181045</v>
       </c>
-      <c r="D58" s="5">
+      <c r="D58" s="6">
         <v>-2.1163790816722896</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F58" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="2:6" ht="162">
-      <c r="B59" s="5">
+    <row r="59" spans="2:6">
+      <c r="B59" s="6">
         <v>-0.72634417697301812</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C59" s="6">
         <v>1.4577886281473607E-2</v>
       </c>
-      <c r="D59" s="5">
+      <c r="D59" s="6">
         <v>-0.7117694054479653</v>
       </c>
-      <c r="F59" s="12" t="s">
+      <c r="F59" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="2:6" ht="162">
-      <c r="B60" s="5">
+    <row r="60" spans="2:6">
+      <c r="B60" s="6">
         <v>-8.0164925928878361E-2</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C60" s="6">
         <v>-6.5619593348120286E-2</v>
       </c>
-      <c r="D60" s="5">
+      <c r="D60" s="6">
         <v>-0.14578154798368725</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="F60" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="61" spans="2:6" ht="162">
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
-      <c r="F61" s="12" t="s">
+    <row r="61" spans="2:6">
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="F61" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="62" spans="2:6" ht="162">
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="F62" s="12" t="s">
+    <row r="62" spans="2:6">
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="F62" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="63" spans="2:6" ht="162">
-      <c r="B63" s="5">
+    <row r="63" spans="2:6">
+      <c r="B63" s="6">
         <v>-0.90902576707244931</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C63" s="6">
         <v>-0.32958545611703371</v>
       </c>
-      <c r="D63" s="5">
+      <c r="D63" s="6">
         <v>-1.2386139793506921</v>
       </c>
-      <c r="F63" s="12" t="s">
+      <c r="F63" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="2:6" ht="162">
-      <c r="B64" s="5">
+    <row r="64" spans="2:6">
+      <c r="B64" s="6">
         <v>-3.8503743400800872E-2</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C64" s="6">
         <v>-1.0826693492620887E-2</v>
       </c>
-      <c r="D64" s="5">
+      <c r="D64" s="6">
         <v>-4.9328349758112289E-2</v>
       </c>
-      <c r="F64" s="12" t="s">
+      <c r="F64" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="65" spans="2:6" ht="162">
-      <c r="B65" s="5">
+    <row r="65" spans="2:6">
+      <c r="B65" s="6">
         <v>-0.10571903040126651</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C65" s="6">
         <v>6.0529215043047202E-2</v>
       </c>
-      <c r="D65" s="5">
+      <c r="D65" s="6">
         <v>-4.518718337023131E-2</v>
       </c>
-      <c r="F65" s="12" t="s">
+      <c r="F65" s="4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="66" spans="2:6" ht="162">
-      <c r="B66" s="5">
+    <row r="66" spans="2:6">
+      <c r="B66" s="6">
         <v>-0.10823304310544746</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C66" s="6">
         <v>0.15792420239731664</v>
       </c>
-      <c r="D66" s="5">
+      <c r="D66" s="6">
         <v>4.9692160584632106E-2</v>
       </c>
-      <c r="F66" s="12" t="s">
+      <c r="F66" s="4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="67" spans="2:6" ht="162">
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="12" t="s">
+    <row r="67" spans="2:6">
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="68" spans="2:6" ht="162">
-      <c r="B68" s="5">
+    <row r="68" spans="2:6">
+      <c r="B68" s="6">
         <v>-0.32735893438633035</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C68" s="6">
         <v>-0.25853964718890232</v>
       </c>
-      <c r="D68" s="5">
+      <c r="D68" s="6">
         <v>-0.58589359506374894</v>
       </c>
-      <c r="F68" s="12" t="s">
+      <c r="F68" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="2:6" ht="162">
-      <c r="B69" s="6"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="F69" s="12" t="s">
+    <row r="69" spans="2:6">
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="F69" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="70" spans="2:6" ht="162">
-      <c r="B70" s="5">
+    <row r="70" spans="2:6">
+      <c r="B70" s="6">
         <v>-1.9252629659431351</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C70" s="6">
         <v>9.063094726615617E-2</v>
       </c>
-      <c r="D70" s="5">
+      <c r="D70" s="6">
         <v>-1.8346241726966102</v>
       </c>
-      <c r="F70" s="12" t="s">
+      <c r="F70" s="4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="71" spans="2:6" ht="162">
-      <c r="B71" s="5">
+    <row r="71" spans="2:6">
+      <c r="B71" s="6">
         <v>-1.4781049346009159</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C71" s="6">
         <v>0.50498135300934122</v>
       </c>
-      <c r="D71" s="5">
+      <c r="D71" s="6">
         <v>-0.9731192512890976</v>
       </c>
-      <c r="F71" s="12" t="s">
+      <c r="F71" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="72" spans="2:6" ht="162">
-      <c r="B72" s="5">
+    <row r="72" spans="2:6">
+      <c r="B72" s="6">
         <v>-1.4036268380538932</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C72" s="6">
         <v>0.22325651254074685</v>
       </c>
-      <c r="D72" s="5">
+      <c r="D72" s="6">
         <v>-1.1803755682145809</v>
       </c>
-      <c r="F72" s="12" t="s">
+      <c r="F72" s="4" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="73" spans="2:6" ht="162">
-      <c r="B73" s="5">
+    <row r="73" spans="2:6">
+      <c r="B73" s="6">
         <v>-0.90902576707244931</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C73" s="6">
         <v>-4.7104663356782428E-2</v>
       </c>
-      <c r="D73" s="5">
+      <c r="D73" s="6">
         <v>-0.95611884302475136</v>
       </c>
-      <c r="F73" s="12" t="s">
+      <c r="F73" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="74" spans="2:6" ht="162">
-      <c r="B74" s="6"/>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="F74" s="12" t="s">
+    <row r="74" spans="2:6">
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="F74" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="75" spans="2:6" ht="162">
-      <c r="B75" s="5">
+    <row r="75" spans="2:6">
+      <c r="B75" s="6">
         <v>-3.4230208480657609E-2</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C75" s="6">
         <v>7.4317499528680386E-2</v>
       </c>
-      <c r="D75" s="5">
+      <c r="D75" s="6">
         <v>4.008887009564166E-2</v>
       </c>
-      <c r="F75" s="12" t="s">
+      <c r="F75" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="76" spans="2:6" ht="162">
-      <c r="B76" s="5">
+    <row r="76" spans="2:6">
+      <c r="B76" s="6">
         <v>7.4737034056865159E-2</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C76" s="6">
         <v>-2.5385413663546075E-2</v>
       </c>
-      <c r="D76" s="5">
+      <c r="D76" s="6">
         <v>4.9353543474047079E-2</v>
       </c>
-      <c r="F76" s="12" t="s">
+      <c r="F76" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="77" spans="2:6" ht="162">
-      <c r="B77" s="5">
+    <row r="77" spans="2:6">
+      <c r="B77" s="6">
         <v>-1.1719352992845236</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C77" s="6">
         <v>-0.44352880842387066</v>
       </c>
-      <c r="D77" s="5">
+      <c r="D77" s="6">
         <v>-1.6154460919688214</v>
       </c>
-      <c r="F77" s="12" t="s">
+      <c r="F77" s="4" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="78" spans="2:6" ht="162">
-      <c r="B78" s="6"/>
-      <c r="C78" s="6"/>
-      <c r="D78" s="5">
+    <row r="78" spans="2:6">
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="6">
         <v>-4.9336138120977875</v>
       </c>
-      <c r="F78" s="12" t="s">
+      <c r="F78" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="79" spans="2:6" ht="162">
-      <c r="B79" s="5">
+    <row r="79" spans="2:6">
+      <c r="B79" s="6">
         <v>-2.4693310102934105</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C79" s="6">
         <v>-1.8975046625198111E-2</v>
       </c>
-      <c r="D79" s="5">
+      <c r="D79" s="6">
         <v>-2.4880096088241901</v>
       </c>
-      <c r="F79" s="12" t="s">
+      <c r="F79" s="4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="80" spans="2:6" ht="162">
-      <c r="B80" s="5">
+    <row r="80" spans="2:6">
+      <c r="B80" s="6">
         <v>-2.9464522650130731</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C80" s="6">
         <v>-5.9780251840064302E-2</v>
       </c>
-      <c r="D80" s="5">
+      <c r="D80" s="6">
         <v>-3.0067571031480953</v>
       </c>
-      <c r="F80" s="12" t="s">
+      <c r="F80" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="81" spans="2:6" ht="162">
-      <c r="B81" s="5">
-        <v>-4.3362278021129352E-2</v>
-      </c>
-      <c r="C81" s="5">
-        <v>-0.1308020105693708</v>
-      </c>
-      <c r="D81" s="5">
-        <v>-0.17416127977666207</v>
-      </c>
-      <c r="F81" s="12" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" ht="162">
-      <c r="B82" s="5">
-        <v>-0.1044674604229594</v>
-      </c>
-      <c r="C82" s="5">
-        <v>9.5857177384790049E-2</v>
-      </c>
-      <c r="D82" s="5">
-        <v>-8.6087236395844258E-3</v>
-      </c>
-      <c r="F82" s="12" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" ht="162">
-      <c r="B83" s="5">
+    <row r="81" spans="2:6">
+      <c r="B81" s="6">
         <v>-0.30696577574448725</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C81" s="6">
         <v>2.7860098289679058E-2</v>
       </c>
-      <c r="D83" s="5">
+      <c r="D81" s="6">
         <v>-0.27910517638973431</v>
       </c>
-      <c r="F83" s="12" t="s">
+      <c r="F81" s="4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="84" spans="2:6" ht="162">
-      <c r="B84" s="5">
+    <row r="82" spans="2:6">
+      <c r="B82" s="6">
         <v>-9.7032851216173555E-2</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C82" s="6">
         <v>-8.8222130202943116E-2</v>
       </c>
-      <c r="D84" s="5">
+      <c r="D82" s="6">
         <v>-0.18525520290728892</v>
       </c>
-      <c r="F84" s="12" t="s">
+      <c r="F82" s="4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="85" spans="2:6" ht="162">
-      <c r="B85" s="5">
+    <row r="83" spans="2:6">
+      <c r="B83" s="6">
         <v>-2.5662410233014672</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C83" s="6">
         <v>-8.3377360641232912E-2</v>
       </c>
-      <c r="D85" s="5">
+      <c r="D83" s="6">
         <v>-2.6491830782532682</v>
       </c>
-      <c r="F85" s="12" t="s">
+      <c r="F83" s="4" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="86" spans="2:6" ht="162">
-      <c r="B86" s="5">
+    <row r="84" spans="2:6">
+      <c r="B84" s="6">
         <v>-3.6454222693490919</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C84" s="6">
         <v>-0.50830085899886401</v>
       </c>
-      <c r="D86" s="5">
+      <c r="D84" s="6">
         <v>-4.1554625617141436</v>
       </c>
-      <c r="F86" s="12" t="s">
+      <c r="F84" s="4" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="87" spans="2:6" ht="162">
-      <c r="B87" s="5">
+    <row r="85" spans="2:6">
+      <c r="B85" s="6">
         <v>-2.5150885008540858</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C85" s="6">
         <v>-1.1351480959786329</v>
       </c>
-      <c r="D87" s="5">
+      <c r="D85" s="6">
         <v>-3.6548602111449586</v>
       </c>
-      <c r="F87" s="12" t="s">
+      <c r="F85" s="4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="88" spans="2:6" ht="162">
-      <c r="B88" s="6"/>
-      <c r="C88" s="6"/>
-      <c r="D88" s="6"/>
-      <c r="F88" s="12" t="s">
+    <row r="86" spans="2:6">
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="F86" s="4" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="89" spans="2:6" ht="162">
-      <c r="B89" s="6"/>
-      <c r="C89" s="6"/>
-      <c r="D89" s="6"/>
-      <c r="F89" s="12" t="s">
+    <row r="87" spans="2:6">
+      <c r="B87" s="8"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
+      <c r="F87" s="4" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="90" spans="2:6" ht="162">
-      <c r="B90" s="5">
+    <row r="88" spans="2:6">
+      <c r="B88" s="6">
         <v>-0.22135774393160412</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C88" s="6">
         <v>0.20395135734536041</v>
       </c>
-      <c r="D90" s="5">
+      <c r="D88" s="6">
         <v>-1.740471672095012E-2</v>
       </c>
-      <c r="F90" s="12" t="s">
+      <c r="F88" s="4" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="91" spans="2:6" ht="162">
-      <c r="B91" s="6"/>
-      <c r="C91" s="6"/>
-      <c r="D91" s="6"/>
-      <c r="F91" s="12" t="s">
+    <row r="89" spans="2:6">
+      <c r="B89" s="8"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
+      <c r="F89" s="4" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="92" spans="2:6" ht="162">
-      <c r="B92" s="5">
+    <row r="90" spans="2:6">
+      <c r="B90" s="6">
         <v>-2.3782505409460781</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C90" s="6">
         <v>-0.26224367375168622</v>
       </c>
-      <c r="D92" s="5">
+      <c r="D90" s="6">
         <v>-2.6402512573863421</v>
       </c>
-      <c r="F92" s="12" t="s">
+      <c r="F90" s="4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="93" spans="2:6" ht="162">
-      <c r="B93" s="6"/>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
-      <c r="F93" s="12" t="s">
+    <row r="91" spans="2:6">
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+      <c r="F91" s="4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="2:6" ht="162">
-      <c r="B94" s="5">
+    <row r="92" spans="2:6">
+      <c r="B92" s="6">
         <v>-1.3542755076172064</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C92" s="6">
         <v>-0.82094714995130658</v>
       </c>
-      <c r="D94" s="5">
+      <c r="D92" s="6">
         <v>-2.1750803898605011</v>
       </c>
-      <c r="F94" s="12" t="s">
+      <c r="F92" s="4" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="95" spans="2:6" ht="162">
-      <c r="B95" s="6"/>
-      <c r="C95" s="6"/>
-      <c r="D95" s="5">
+    <row r="93" spans="2:6">
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="6">
         <v>-4.53567380342575</v>
       </c>
-      <c r="F95" s="12" t="s">
+      <c r="F93" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="96" spans="2:6" ht="162">
-      <c r="B96" s="5">
+    <row r="94" spans="2:6">
+      <c r="B94" s="6">
         <v>-1.8895474136766004</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C94" s="6">
         <v>-0.16957742772938156</v>
       </c>
-      <c r="D96" s="5">
+      <c r="D94" s="6">
         <v>-2.0591319943983213</v>
       </c>
-      <c r="F96" s="12" t="s">
+      <c r="F94" s="4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="97" spans="2:6" ht="162">
-      <c r="B97" s="5">
+    <row r="95" spans="2:6">
+      <c r="B95" s="6">
         <v>-1.2518470660795045</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C95" s="6">
         <v>-0.33351574974546616</v>
       </c>
-      <c r="D97" s="5">
+      <c r="D95" s="6">
         <v>-1.5854063354121615</v>
       </c>
-      <c r="F97" s="12" t="s">
+      <c r="F95" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="98" spans="2:6" ht="162">
-      <c r="B98" s="6"/>
-      <c r="C98" s="6"/>
-      <c r="D98" s="6"/>
-      <c r="F98" s="12" t="s">
+    <row r="96" spans="2:6">
+      <c r="B96" s="8"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
+      <c r="F96" s="4" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="99" spans="2:6" ht="162">
-      <c r="B99" s="6"/>
-      <c r="C99" s="6"/>
-      <c r="D99" s="6"/>
-      <c r="F99" s="12" t="s">
+    <row r="97" spans="2:6">
+      <c r="B97" s="8"/>
+      <c r="C97" s="8"/>
+      <c r="D97" s="8"/>
+      <c r="F97" s="4" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="100" spans="2:6" ht="162">
-      <c r="B100" s="6"/>
-      <c r="C100" s="6"/>
-      <c r="D100" s="6"/>
-      <c r="F100" s="12" t="s">
+    <row r="98" spans="2:6">
+      <c r="B98" s="8"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8"/>
+      <c r="F98" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="101" spans="2:6" ht="162">
-      <c r="B101" s="5">
-        <v>0.22086506973510289</v>
-      </c>
-      <c r="C101" s="5">
-        <v>7.3317972086553773E-2</v>
-      </c>
-      <c r="D101" s="5">
-        <v>0.29418422571600455</v>
-      </c>
-      <c r="F101" s="12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="102" spans="2:6" ht="162">
-      <c r="B102" s="6"/>
-      <c r="C102" s="6"/>
-      <c r="D102" s="6"/>
-      <c r="F102" s="12" t="s">
+    <row r="99" spans="2:6">
+      <c r="B99" s="8"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+      <c r="F99" s="4" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="103" spans="2:6" ht="162">
-      <c r="B103" s="5">
+    <row r="100" spans="2:6">
+      <c r="B100" s="6">
         <v>-2.4765789529471061E-2</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C100" s="6">
         <v>0.2464243775927728</v>
       </c>
-      <c r="D103" s="5">
+      <c r="D100" s="6">
         <v>0.22165996190507276</v>
       </c>
-      <c r="F103" s="12" t="s">
+      <c r="F100" s="4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="104" spans="2:6" ht="162">
-      <c r="B104" s="5">
+    <row r="101" spans="2:6">
+      <c r="B101" s="6">
         <v>-2.8325089127062362</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C101" s="6">
         <v>-0.50830085899886401</v>
       </c>
-      <c r="D104" s="5">
+      <c r="D101" s="6">
         <v>-3.3425492050712884</v>
       </c>
-      <c r="F104" s="12" t="s">
+      <c r="F101" s="4" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="105" spans="2:6" ht="162">
-      <c r="B105" s="5">
+    <row r="102" spans="2:6">
+      <c r="B102" s="6">
         <v>-0.13621974701798889</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C102" s="6">
         <v>-0.10773670650067757</v>
       </c>
-      <c r="D105" s="5">
+      <c r="D102" s="6">
         <v>-0.24395428411410158</v>
       </c>
-      <c r="F105" s="12" t="s">
+      <c r="F102" s="4" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="106" spans="2:6" ht="162">
-      <c r="B106" s="5">
+    <row r="103" spans="2:6">
+      <c r="B103" s="6">
         <v>0</v>
       </c>
-      <c r="C106" s="5">
+      <c r="C103" s="6">
         <v>0</v>
       </c>
-      <c r="D106" s="5">
+      <c r="D103" s="6">
         <v>0</v>
       </c>
-      <c r="F106" s="12" t="s">
+      <c r="F103" s="4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="110" spans="2:6">
-      <c r="C110" s="5">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B2:D1048576">
     <cfRule type="colorScale" priority="10">
       <colorScale>
@@ -2698,7 +2626,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="58" scale="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="58" scale="35" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="100"/>
@@ -3444,80 +3372,80 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="11">
+      <c r="A7" s="1">
         <v>19</v>
       </c>
-      <c r="B7" s="11">
-        <v>1</v>
-      </c>
-      <c r="C7" s="11">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
         <v>0.26</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="11">
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="1">
         <v>3</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="11">
+      <c r="A8" s="1">
         <v>19</v>
       </c>
-      <c r="B8" s="11">
-        <v>1</v>
-      </c>
-      <c r="C8" s="11">
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
         <v>0.4</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="11">
-        <v>8</v>
-      </c>
-      <c r="H8" s="11" t="s">
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1">
+        <v>8</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="11">
+      <c r="A9" s="1">
         <v>19</v>
       </c>
-      <c r="B9" s="11">
-        <v>1</v>
-      </c>
-      <c r="C9" s="11">
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
         <v>0.43</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="11">
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1">
         <v>5</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="1" t="s">
         <v>112</v>
       </c>
     </row>
@@ -3964,28 +3892,28 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="11">
+      <c r="A27" s="1">
         <v>164</v>
       </c>
-      <c r="B27" s="11">
-        <v>1</v>
-      </c>
-      <c r="C27" s="11">
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
         <v>0.42</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="1">
         <v>0.2</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="1">
         <v>1.01E-3</v>
       </c>
-      <c r="F27" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="11">
+      <c r="F27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="1">
         <v>198</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -4458,28 +4386,28 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="11">
+      <c r="A46" s="1">
         <v>222</v>
       </c>
-      <c r="B46" s="11">
-        <v>1</v>
-      </c>
-      <c r="C46" s="11">
+      <c r="B46" s="1">
+        <v>1</v>
+      </c>
+      <c r="C46" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="D46" s="11">
+      <c r="D46" s="1">
         <v>89.9</v>
       </c>
-      <c r="E46" s="11">
+      <c r="E46" s="1">
         <v>6.3000000000000003E-4</v>
       </c>
-      <c r="F46" s="11">
+      <c r="F46" s="1">
         <v>9.5240000000000005E-2</v>
       </c>
-      <c r="G46" s="11">
+      <c r="G46" s="1">
         <v>143610</v>
       </c>
-      <c r="H46" s="11" t="s">
+      <c r="H46" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -4640,28 +4568,28 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="11">
+      <c r="A53" s="1">
         <v>240</v>
       </c>
-      <c r="B53" s="11">
-        <v>1</v>
-      </c>
-      <c r="C53" s="11">
+      <c r="B53" s="1">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1">
         <v>1.1100000000000001</v>
       </c>
-      <c r="D53" s="11">
+      <c r="D53" s="1">
         <v>11000</v>
       </c>
-      <c r="E53" s="11">
+      <c r="E53" s="1">
         <v>1.95E-2</v>
       </c>
-      <c r="F53" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G53" s="11">
+      <c r="F53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" s="1">
         <v>564103</v>
       </c>
-      <c r="H53" s="11" t="s">
+      <c r="H53" s="1" t="s">
         <v>57</v>
       </c>
     </row>
@@ -4848,54 +4776,54 @@
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="11">
+      <c r="A61" s="1">
         <v>295</v>
       </c>
-      <c r="B61" s="11">
-        <v>1</v>
-      </c>
-      <c r="C61" s="11">
+      <c r="B61" s="1">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1">
         <v>0.69</v>
       </c>
-      <c r="D61" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E61" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F61" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G61" s="11">
+      <c r="D61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G61" s="1">
         <v>0</v>
       </c>
-      <c r="H61" s="11" t="s">
+      <c r="H61" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="11">
+      <c r="A62" s="1">
         <v>295</v>
       </c>
-      <c r="B62" s="11">
-        <v>1</v>
-      </c>
-      <c r="C62" s="11">
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1">
         <v>0.77</v>
       </c>
-      <c r="D62" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F62" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G62" s="11">
+      <c r="D62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="1">
         <v>0</v>
       </c>
-      <c r="H62" s="11" t="s">
+      <c r="H62" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -5290,28 +5218,28 @@
       </c>
     </row>
     <row r="78" spans="1:8">
-      <c r="A78" s="11">
+      <c r="A78" s="1">
         <v>353</v>
       </c>
-      <c r="B78" s="11">
-        <v>1</v>
-      </c>
-      <c r="C78" s="11">
+      <c r="B78" s="1">
+        <v>1</v>
+      </c>
+      <c r="C78" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="D78" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E78" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F78" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G78" s="11">
+      <c r="D78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G78" s="1">
         <v>2</v>
       </c>
-      <c r="H78" s="11" t="s">
+      <c r="H78" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -6018,28 +5946,28 @@
       </c>
     </row>
     <row r="106" spans="1:8">
-      <c r="A106" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B106" s="11">
-        <v>1</v>
-      </c>
-      <c r="C106" s="11">
+      <c r="A106" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B106" s="1">
+        <v>1</v>
+      </c>
+      <c r="C106" s="1">
         <v>0.47</v>
       </c>
-      <c r="D106" s="11">
+      <c r="D106" s="1">
         <v>884</v>
       </c>
-      <c r="E106" s="11">
+      <c r="E106" s="1">
         <v>5.1500000000000001E-3</v>
       </c>
-      <c r="F106" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G106" s="11">
+      <c r="F106" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G106" s="1">
         <v>171650</v>
       </c>
-      <c r="H106" s="11" t="s">
+      <c r="H106" s="1" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>